<commit_message>
squashed bug where double CO2 was sent to CCS
</commit_message>
<xml_diff>
--- a/data/steel/birat_factories.xlsx
+++ b/data/steel/birat_factories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4116917C-A15D-D044-A153-D04CE3F34535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C04D6-9BE9-C146-8949-4CD9908AF917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="680" windowWidth="26520" windowHeight="17240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="760" windowWidth="26520" windowHeight="17240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base chains" sheetId="9" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>CO2__emitted</t>
   </si>
   <si>
-    <t>secondary fuel</t>
-  </si>
-  <si>
     <t>energy</t>
   </si>
   <si>
@@ -158,10 +155,13 @@
     <t>meta-notes</t>
   </si>
   <si>
-    <t>includes both CO2 of steel production and electricity (but not CO2 from electricity needed for the CO2 plant)</t>
-  </si>
-  <si>
     <t>fossil fuel</t>
+  </si>
+  <si>
+    <t>secondary fuel__TGR</t>
+  </si>
+  <si>
+    <t>includes  CO2 from electricity generated for steel plant (but not CO2 from electricity needed for the CO2 plant)</t>
   </si>
 </sst>
 </file>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1228,7 +1228,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1260,9 +1260,9 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
@@ -1284,12 +1284,12 @@
         <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1330,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>30</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1388,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>

</xml_diff>